<commit_message>
Update code from pycharm (#2)
</commit_message>
<xml_diff>
--- a/abner/Config_Files/Scheduler.xlsx
+++ b/abner/Config_Files/Scheduler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b15f2988ffa366a8/Documents/WELLS/ND_152N_101W_20241004_LAS_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b15f2988ffa366a8/Documents/WELLS/Junk_3Wells/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="297" documentId="11_F25DC773A252ABDACC1048FFB9DA68485ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{697370F8-F778-4180-B558-655CAE694AEF}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="11_F25DC773A252ABDACC1048FFB9DA68485ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E16F2B3-932D-47B0-8A1E-DCFCA3C78933}"/>
   <bookViews>
-    <workbookView xWindow="33930" yWindow="2720" windowWidth="23070" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19500" yWindow="3560" windowWidth="16840" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
     <t>Casing_Check</t>
   </si>
   <si>
-    <t>Update_Project_WellInfo</t>
+    <t>WellInfo_Update</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>